<commit_message>
fix: default value of eamilVerified is 1
</commit_message>
<xml_diff>
--- a/public/excel/user.xlsx
+++ b/public/excel/user.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeshrz/Projects/SDUOJ/sduoj-manage/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7000451-8D46-9244-B6B4-88F7804B171A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB35B398-4888-F04D-A01C-2FF5AB13EF6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="4720" windowWidth="36280" windowHeight="22140" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
+    <workbookView xWindow="14920" yWindow="460" windowWidth="36280" windowHeight="20960" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否通过邮箱验证，0表示不验证，1表示通过验证，默认为0</t>
+    <t>是否需要进行邮箱验证，1表示已通过邮箱验证，0表示需要用户邮箱验证，默认为1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -495,7 +495,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
bugfix: a series of bugs (#37)
* fix: default value of eamilVerified is 1

* feat: show private contest tag

* fix: set to correct problem description when editing contests

* fix: correctly delete manager group
</commit_message>
<xml_diff>
--- a/public/excel/user.xlsx
+++ b/public/excel/user.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeshrz/Projects/SDUOJ/sduoj-manage/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7000451-8D46-9244-B6B4-88F7804B171A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB35B398-4888-F04D-A01C-2FF5AB13EF6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="4720" windowWidth="36280" windowHeight="22140" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
+    <workbookView xWindow="14920" yWindow="460" windowWidth="36280" windowHeight="20960" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否通过邮箱验证，0表示不验证，1表示通过验证，默认为0</t>
+    <t>是否需要进行邮箱验证，1表示已通过邮箱验证，0表示需要用户邮箱验证，默认为1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -495,7 +495,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
refactor: set email field as unnecessary
</commit_message>
<xml_diff>
--- a/public/excel/user.xlsx
+++ b/public/excel/user.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeshrz/Projects/SDUOJ/sduoj-manage/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB35B398-4888-F04D-A01C-2FF5AB13EF6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50D8B56-91C5-2248-AF68-2E357F0DAEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14920" yWindow="460" windowWidth="36280" windowHeight="20960" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,10 +52,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>emailVerified</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>phone</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,10 +73,6 @@
   </si>
   <si>
     <t>必填，密码不能为空，长度必须在6-32位之间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>必填，邮箱不能为空</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -97,7 +89,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否需要进行邮箱验证，1表示已通过邮箱验证，0表示需要用户邮箱验证，默认为1</t>
+    <t>选填，邮箱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -492,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04E3C33-3AF4-EA44-8D06-C096B553D7E7}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -505,7 +497,7 @@
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -527,76 +519,70 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="153">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="153">
-      <c r="A2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:7">
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:7">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:7">
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:7">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:7">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:7">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:7">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:7">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:7">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:7">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:7">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:7">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:7">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:7">
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="3:3">

</xml_diff>

<commit_message>
feat: add banThirdParty and banEmailUpdate
</commit_message>
<xml_diff>
--- a/public/excel/user.xlsx
+++ b/public/excel/user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeshrz/Projects/SDUOJ/sduoj-manage/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50D8B56-91C5-2248-AF68-2E357F0DAEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7166A3FE-8077-6440-AD84-3B67E2D6E0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="460" windowWidth="36280" windowHeight="20960" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20960" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,6 +90,20 @@
   </si>
   <si>
     <t>选填，邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>banEmailUpdate</t>
+  </si>
+  <si>
+    <t>选填，0或1，1表示禁止更改邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>banThirdParty</t>
+  </si>
+  <si>
+    <t>选填，0或1，1表示禁止使用第三方登录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -484,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04E3C33-3AF4-EA44-8D06-C096B553D7E7}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -497,7 +511,7 @@
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -519,8 +533,14 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="153">
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="153">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -542,47 +562,53 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="3:3">

</xml_diff>

<commit_message>
refactor: email field's biz in user module (#44)
* refactor: set email field as unnecessary

* feat: add banThirdParty and banEmailUpdate

* feat: search user by any key

* fix: add select transfer

* fix: record searchKey in url

* update gitignore

* fix: get searchKey from variable, not router query params
</commit_message>
<xml_diff>
--- a/public/excel/user.xlsx
+++ b/public/excel/user.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeshrz/Projects/SDUOJ/sduoj-manage/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB35B398-4888-F04D-A01C-2FF5AB13EF6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7166A3FE-8077-6440-AD84-3B67E2D6E0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="460" windowWidth="36280" windowHeight="20960" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20960" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,10 +52,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>emailVerified</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>phone</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,10 +73,6 @@
   </si>
   <si>
     <t>必填，密码不能为空，长度必须在6-32位之间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>必填，邮箱不能为空</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -97,7 +89,21 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否需要进行邮箱验证，1表示已通过邮箱验证，0表示需要用户邮箱验证，默认为1</t>
+    <t>选填，邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>banEmailUpdate</t>
+  </si>
+  <si>
+    <t>选填，0或1，1表示禁止更改邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>banThirdParty</t>
+  </si>
+  <si>
+    <t>选填，0或1，1表示禁止使用第三方登录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -492,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04E3C33-3AF4-EA44-8D06-C096B553D7E7}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -505,7 +511,7 @@
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -528,75 +534,81 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="153">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="153">
-      <c r="A2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:9">
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="3:3">

</xml_diff>

<commit_message>
feat: add ban-updating-info feature for user
</commit_message>
<xml_diff>
--- a/public/excel/user.xlsx
+++ b/public/excel/user.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeshrz/Projects/SDUOJ/sduoj-manage/public/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TTTT\Desktop\tempProjects\sduoj-manage\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7166A3FE-8077-6440-AD84-3B67E2D6E0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BE4997-C427-4F75-99C3-402DBA36CE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20960" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
+    <workbookView xWindow="4180" yWindow="4180" windowWidth="29730" windowHeight="8710" xr2:uid="{707A7C23-4E45-0241-BA3B-C07BEB678DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,34 +76,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>样例行，不可删除
+    <t>选填，学号长度在20位之内</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.女, 1.男, 2.问号，默认为2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选填，邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>banEmailUpdate</t>
+  </si>
+  <si>
+    <t>banThirdParty</t>
+  </si>
+  <si>
+    <t>banInfoUpdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选填，0或1，1表示禁止使用第三方登录，默认为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选填，0或1，1表示禁止更改邮箱，默认为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选填，0或1，1表示禁止更改个人信息，默认为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>此行为样例，不可删除。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="4"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 必填，用户名必须由英文、数字、'_'构成，且长度为4~16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选填，学号长度在20位之内</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.女, 1.男, 2.问号，默认为2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选填，邮箱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>banEmailUpdate</t>
-  </si>
-  <si>
-    <t>选填，0或1，1表示禁止更改邮箱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>banThirdParty</t>
-  </si>
-  <si>
-    <t>选填，0或1，1表示禁止使用第三方登录</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -111,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +173,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,18 +215,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -498,139 +549,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04E3C33-3AF4-EA44-8D06-C096B553D7E7}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.3046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.61328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.23046875" style="1" customWidth="1"/>
+    <col min="4" max="7" width="11.07421875" style="1"/>
+    <col min="8" max="8" width="11.69140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.15234375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.07421875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="153">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3">
-      <c r="C22" s="1"/>
+      <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>